<commit_message>
20170601 Route 1 Fixes.
</commit_message>
<xml_diff>
--- a/route/timepoints/timepoints_1.xlsx
+++ b/route/timepoints/timepoints_1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="21">
   <si>
     <t>Timepoints for Driver Position 1</t>
   </si>
@@ -453,7 +453,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -553,16 +553,16 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -609,30 +609,30 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -665,44 +665,44 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -721,267 +721,169 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D22" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D26" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="4" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C30" t="s">
         <v>17</v>
       </c>
       <c r="D30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" t="s">
-        <v>10</v>
-      </c>
-      <c r="B32" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" t="s">
-        <v>19</v>
-      </c>
-      <c r="B34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" t="s">
-        <v>19</v>
-      </c>
-      <c r="B36" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" t="s">
-        <v>17</v>
-      </c>
-      <c r="D36" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" t="s">
-        <v>19</v>
-      </c>
-      <c r="B38" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" t="s">
-        <v>17</v>
-      </c>
-      <c r="D38" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>